<commit_message>
Added upated DT results with demographics removed
</commit_message>
<xml_diff>
--- a/Model Performance Tracking.xlsx
+++ b/Model Performance Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\James Data\Admin\Apprenticeship\l7hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF8AED-B6C6-4C6F-8C23-0E1B3C26A251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE90673-B701-4F19-A623-13BEDF58A19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$20</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Model</t>
   </si>
@@ -117,26 +117,41 @@
     <t>Fuller dataset, Best model{'n_estimators': 200, 'learning_rate': 0.1, 'max_depth': 3}</t>
   </si>
   <si>
-    <t>No demographic data, No hyperparamter tuning,  train/test split done using train_test_split with test_size=0.3,stratify=y,random_state=42</t>
-  </si>
-  <si>
-    <t>No demographic data,  RandomSearchCV,  train/test split done using train_test_split with test_size=0.3,stratify=y,random_state=42</t>
-  </si>
-  <si>
     <t>RandomSearchCV</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Best model{'criterion': 'gini', 'max_depth': 15, 'max_features': 8, 'min_samples_leaf': 16, 'min_samples_split': 5}</t>
+  </si>
+  <si>
+    <t>Removed demographics Best model {'criterion': 'entropy', 'max_depth': 20, 'max_features': 8, 'min_samples_leaf': 8, 'min_samples_split': 5}</t>
+  </si>
+  <si>
+    <t>Fuller dataset, Best model {'criterion': 'entropy', 'max_depth': 20, 'max_features': 8, 'min_samples_leaf': 8, 'min_samples_split': 5}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,11 +174,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -480,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>0.96</v>
@@ -1071,10 +1090,40 @@
         <v>0.89</v>
       </c>
       <c r="I20" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E21">
+        <v>0.77</v>
+      </c>
+      <c r="F21">
+        <v>0.54</v>
+      </c>
+      <c r="G21">
+        <v>0.63</v>
+      </c>
+      <c r="H21">
+        <v>0.89</v>
+      </c>
+      <c r="I21" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I20" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
     <sortCondition descending="1" ref="F2:F12"/>
   </sortState>
@@ -1084,62 +1133,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45B5749-C934-49B5-8A31-D5E0E64BC1FF}">
-  <dimension ref="B13:H14"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="2:8" ht="285" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3">
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="247.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.81</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.59</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="346.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5">
         <v>0.89</v>
       </c>
-      <c r="D13" s="3">
+      <c r="C4" s="5">
         <v>0.97</v>
       </c>
-      <c r="E13" s="3">
-        <v>0.76</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="D4" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="E4" s="5">
         <v>0.54</v>
       </c>
-      <c r="G13" s="3">
+      <c r="F4" s="5">
         <v>0.63</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="285" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.97</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.76</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.63</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added in DT result with no demogs and no tuning
</commit_message>
<xml_diff>
--- a/Model Performance Tracking.xlsx
+++ b/Model Performance Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\James Data\Admin\Apprenticeship\l7hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE90673-B701-4F19-A623-13BEDF58A19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F4094F-3D98-46D0-9A85-4F31B716EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$21</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Model</t>
   </si>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,8 +1122,36 @@
         <v>30</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E22">
+        <v>0.78</v>
+      </c>
+      <c r="F22">
+        <v>0.54</v>
+      </c>
+      <c r="G22">
+        <v>0.64</v>
+      </c>
+      <c r="H22">
+        <v>0.89</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I20" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
     <sortCondition descending="1" ref="F2:F12"/>
   </sortState>

</xml_diff>